<commit_message>
updated notebooks with analysis that follow structure of the paper delimited over the holiday
</commit_message>
<xml_diff>
--- a/data/final/factor_analysis_gpt-3.5-turbo.xlsx
+++ b/data/final/factor_analysis_gpt-3.5-turbo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/076a438a88ad6cf7/trabalho/repositorios/mfv_llm/data/final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_262949D406446A0F62355476585DCE3A87472156" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B4D1D9-FAF8-E446-86FF-80A10587CEA7}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_262949D406446A0F62355476585DCE3A87472156" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCD9BC84-458C-467B-9F4F-61F1F0AFF9D8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,6 +293,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -339,7 +340,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -365,6 +366,12 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -667,12 +674,12 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -739,7 +746,7 @@
         <v>-0.15969010749102949</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -774,7 +781,7 @@
         <v>-5.7936202189778428E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -809,7 +816,7 @@
         <v>7.3818535823748421E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -844,7 +851,7 @@
         <v>6.7331118477214858E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -879,7 +886,7 @@
         <v>9.7822102919107451E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -914,7 +921,7 @@
         <v>0.1057653624249644</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -949,7 +956,7 @@
         <v>4.6235901802747892E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -984,7 +991,7 @@
         <v>0.1109972455098388</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>6.8846780089023063E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>3.6541344087883433E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1089,7 +1096,7 @@
         <v>0.1112922941731745</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>-4.1766616181290753E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>-2.7599564421804151E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>-7.5264981366538281E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>-4.4624311657038222E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>9.2299580356197702E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1299,7 +1306,7 @@
         <v>-8.7077208040140085E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>1.415080947181417E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>4.359004821092384E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1404,7 +1411,7 @@
         <v>1.303587934317489E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>0.13927752343831951</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1474,7 +1481,7 @@
         <v>0.29902788205861169</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1509,7 +1516,7 @@
         <v>0.39192876537984062</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>0.66776009600998343</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>0.52260945797413172</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1614,7 +1621,7 @@
         <v>0.94313288441812826</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1649,7 +1656,7 @@
         <v>0.17560142422954059</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1684,7 +1691,7 @@
         <v>0.98073982707890606</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1719,7 +1726,7 @@
         <v>0.31470015715878108</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1754,7 +1761,7 @@
         <v>7.4474882825213917E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1789,7 +1796,7 @@
         <v>6.2901567823840576E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1824,7 +1831,7 @@
         <v>6.7869450501577916E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>-6.514034811222473E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1894,7 +1901,7 @@
         <v>-2.2313714913485948E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1929,7 +1936,7 @@
         <v>-9.5259933499668659E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1964,7 +1971,7 @@
         <v>-8.5273661928381511E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1999,7 +2006,7 @@
         <v>-0.25441271805692511</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2034,7 +2041,7 @@
         <v>-0.12240369452635801</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2069,7 +2076,7 @@
         <v>-0.13729438868014199</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2104,7 +2111,7 @@
         <v>-0.21503032847744041</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2139,7 +2146,7 @@
         <v>9.0275260374703473E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2174,7 +2181,7 @@
         <v>-3.7806956719513021E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2209,7 +2216,7 @@
         <v>-3.6364147726007552E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2244,7 +2251,7 @@
         <v>-8.6532818257027674E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2279,7 +2286,7 @@
         <v>2.9578604958615761E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>0.14260181434372099</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2349,7 +2356,7 @@
         <v>0.12763567808439821</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2384,7 +2391,7 @@
         <v>0.15644493915355251</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2419,7 +2426,7 @@
         <v>-2.1192400878290291E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2454,7 +2461,7 @@
         <v>-5.1826229206891228E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2489,7 +2496,7 @@
         <v>-5.3731274259148858E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2524,7 +2531,7 @@
         <v>1.0521153402729791E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2559,7 +2566,7 @@
         <v>8.8725220117303327E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2594,7 +2601,7 @@
         <v>-2.7480679435638328E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2629,7 +2636,7 @@
         <v>-3.6745502391059622E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2664,7 +2671,7 @@
         <v>0.1007344681956481</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>-1.725236520363874E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2734,7 +2741,7 @@
         <v>-5.5098984886181243E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>4.6733339734800192E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2804,7 +2811,7 @@
         <v>-8.6882305527466522E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2839,7 +2846,7 @@
         <v>3.3701896705125869E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2874,7 +2881,7 @@
         <v>-4.7975610938534252E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2909,7 +2916,7 @@
         <v>-7.6632392259639234E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2944,7 +2951,7 @@
         <v>2.571416048955107E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2979,7 +2986,7 @@
         <v>-2.006849685555041E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3014,7 +3021,7 @@
         <v>6.6829825975466522E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3049,7 +3056,7 @@
         <v>-4.6216161166728893E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3086,10 +3093,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:K69">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0.3</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
-      <formula>0.6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>